<commit_message>
fix: - added shoe materials - edited colors
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/перчатки_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/перчатки_по каждому размеру.xlsx
@@ -993,7 +993,7 @@
     <t>КИРГИЗИЯ</t>
   </si>
   <si>
-    <t>НЕ КЛАССИФИЦИРОВАНО</t>
+    <t>СВЕТЛО-ЖЕЛТЫЙ</t>
   </si>
   <si>
     <t>70-72</t>
@@ -1002,13 +1002,13 @@
     <t>КИРИБАТИ</t>
   </si>
   <si>
-    <t>НЕ ОПРЕДЕЛЕНО</t>
+    <t>ТЕМНО-ЖЕЛТЫЙ</t>
   </si>
   <si>
     <t>72-74</t>
   </si>
   <si>
-    <t>СВЕТЛО-ЖЕЛТЫЙ</t>
+    <t>ЛИЛОВЫЙ</t>
   </si>
   <si>
     <t>74-76</t>
@@ -1017,7 +1017,7 @@
     <t>КОКОСОВЫЕ ОСТРОВА (ОСТРОВА КИЛИНГ)</t>
   </si>
   <si>
-    <t>ТЕМНО-ЖЕЛТЫЙ</t>
+    <t>СЕРЫЙ/ЗЕЛЕНЫЙ</t>
   </si>
   <si>
     <t>76-78</t>
@@ -1026,7 +1026,7 @@
     <t>КОЛУМБИЯ</t>
   </si>
   <si>
-    <t>ЛИЛОВЫЙ</t>
+    <t>СИНЕ-ЗЕЛЕНЫЙ</t>
   </si>
   <si>
     <t>78-80</t>
@@ -1035,7 +1035,7 @@
     <t>КОМОРСКИЕ ОСТРОВА</t>
   </si>
   <si>
-    <t>СЕРЫЙ/ЗЕЛЕНЫЙ</t>
+    <t>БЕЛО-ГОЛУБОЙ</t>
   </si>
   <si>
     <t>80-82</t>
@@ -1044,7 +1044,7 @@
     <t>КОСТА-РИКА</t>
   </si>
   <si>
-    <t>СИНЕ-ЗЕЛЕНЫЙ</t>
+    <t>БЕЛО-СИНИЙ</t>
   </si>
   <si>
     <t>82-84</t>
@@ -1053,7 +1053,7 @@
     <t>КОТ-Д'ИВУАР</t>
   </si>
   <si>
-    <t>БЕЛО-ГОЛУБОЙ</t>
+    <t>СВЕТЛО-ГОЛУБОЙ</t>
   </si>
   <si>
     <t>84-86</t>
@@ -1062,7 +1062,7 @@
     <t>КУБА</t>
   </si>
   <si>
-    <t>БЕЛО-СИНИЙ</t>
+    <t>ЗЕЛЕНЫЙ МЕЛАНЖ</t>
   </si>
   <si>
     <t>86-88</t>
@@ -1071,7 +1071,7 @@
     <t>КУВЕЙТ</t>
   </si>
   <si>
-    <t>СВЕТЛО-ГОЛУБОЙ</t>
+    <t>ЖЕЛТЫЙ МЕЛАНЖ</t>
   </si>
   <si>
     <t>88-90</t>
@@ -1080,7 +1080,7 @@
     <t>ЛАОССКАЯ НАРОДНАЯ ДЕМОКРАТИЧЕСКАЯ РЕСПУБЛИКА</t>
   </si>
   <si>
-    <t>ЗЕЛЕНЫЙ МЕЛАНЖ</t>
+    <t>СИНИЙ МЕЛАНЖ</t>
   </si>
   <si>
     <t>90-92</t>
@@ -1089,7 +1089,7 @@
     <t>ЛАТВИЯ</t>
   </si>
   <si>
-    <t>ЖЕЛТЫЙ МЕЛАНЖ</t>
+    <t>КРАСНЫЙ МЕЛАНЖ</t>
   </si>
   <si>
     <t>92-94</t>
@@ -1098,7 +1098,7 @@
     <t>ЛЕСОТО</t>
   </si>
   <si>
-    <t>СИНИЙ МЕЛАНЖ</t>
+    <t>РОЗОВЫЙ МЕЛАНЖ</t>
   </si>
   <si>
     <t>94-96</t>
@@ -1107,7 +1107,7 @@
     <t>ЛИБЕРИЯ</t>
   </si>
   <si>
-    <t>КРАСНЫЙ МЕЛАНЖ</t>
+    <t>ФИОЛЕТОВЫЙ МЕЛАНЖ</t>
   </si>
   <si>
     <t>96-98</t>
@@ -1116,7 +1116,7 @@
     <t>ЛИВАН</t>
   </si>
   <si>
-    <t>РОЗОВЫЙ МЕЛАНЖ</t>
+    <t>ЖЕЛТО-ЗЕЛЕНЫЙ</t>
   </si>
   <si>
     <t>98-100</t>
@@ -1125,7 +1125,7 @@
     <t>ЛИВИЯ</t>
   </si>
   <si>
-    <t>ФИОЛЕТОВЫЙ МЕЛАНЖ</t>
+    <t>МЕЛАНЖ</t>
   </si>
   <si>
     <t>50-56</t>
@@ -1134,16 +1134,10 @@
     <t>ЛИТВА</t>
   </si>
   <si>
-    <t>ЖЕЛТО-ЗЕЛЕНЫЙ</t>
-  </si>
-  <si>
     <t>56-62</t>
   </si>
   <si>
     <t>ЛИХТЕНШТЕЙН</t>
-  </si>
-  <si>
-    <t>МЕЛАНЖ</t>
   </si>
   <si>
     <t>62-68</t>
@@ -15709,7 +15703,11 @@
       <formula1>'Справочники'!$F$2:$F$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G7:G1045" type="textLength">
+    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N7:N1045" type="list">
+      <formula1>'Справочники'!$I$2:$I$243</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J1045" type="textLength">
       <formula1>100</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -15717,20 +15715,12 @@
       <formula1>'Справочники'!$J$2:$J$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N7:N1045" type="list">
-      <formula1>'Справочники'!$I$2:$I$243</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G7:G1045" type="textLength">
+      <formula1>100</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I7:I1045" type="list">
       <formula1>'Справочники'!$G$2:$G$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F1:F3 F7:F1045" type="list">
-      <formula1>'Справочники'!$D$2:$D$51</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J1045" type="textLength">
-      <formula1>100</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 G6:H6" type="textLength">
@@ -15747,6 +15737,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B7:B45" type="textLength">
       <formula1>129</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" imeMode="noControl" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F1:F3 F7:F1045" type="list">
+      <formula1>'Справочники'!$D$2:$D$51</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -17116,831 +17110,961 @@
       </c>
     </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="111">
-      <c r="E111" s="1" t="s">
+      <c r="E111" t="n"/>
+      <c r="H111" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="H111" s="1" t="s">
+      <c r="I111" s="32" t="s">
         <v>344</v>
       </c>
-      <c r="I111" s="32" t="s">
+    </row>
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="112">
+      <c r="E112" t="n"/>
+      <c r="H112" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="112">
-      <c r="E112" s="1" t="s">
+      <c r="I112" s="32" t="s">
         <v>346</v>
       </c>
-      <c r="H112" s="1" t="s">
+    </row>
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="113">
+      <c r="E113" s="1" t="n"/>
+      <c r="H113" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="I112" s="32" t="s">
+      <c r="I113" s="32" t="s">
         <v>348</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="113">
-      <c r="H113" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="114">
+      <c r="E114" s="1" t="n"/>
+      <c r="H114" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="I113" s="32" t="s">
+      <c r="I114" s="32" t="s">
         <v>350</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="114">
-      <c r="H114" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="115">
+      <c r="E115" s="1" t="n"/>
+      <c r="H115" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="I114" s="32" t="s">
+      <c r="I115" s="32" t="s">
         <v>352</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="115">
-      <c r="H115" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="116">
+      <c r="E116" s="1" t="n"/>
+      <c r="H116" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="I115" s="32" t="s">
+      <c r="I116" s="32" t="s">
         <v>354</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="116">
-      <c r="H116" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="117">
+      <c r="E117" s="1" t="n"/>
+      <c r="H117" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="I116" s="32" t="s">
+      <c r="I117" s="32" t="s">
         <v>356</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="117">
-      <c r="H117" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="118">
+      <c r="E118" s="1" t="n"/>
+      <c r="H118" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="I117" s="32" t="s">
+      <c r="I118" s="32" t="s">
         <v>358</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="118">
-      <c r="H118" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="119">
+      <c r="E119" s="1" t="n"/>
+      <c r="H119" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="I118" s="32" t="s">
+      <c r="I119" s="32" t="s">
         <v>360</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="119">
-      <c r="H119" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="120">
+      <c r="E120" s="1" t="n"/>
+      <c r="H120" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="I119" s="32" t="s">
+      <c r="I120" s="32" t="s">
         <v>362</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="120">
-      <c r="H120" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="121">
+      <c r="E121" s="1" t="n"/>
+      <c r="H121" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="I120" s="32" t="s">
+      <c r="I121" s="32" t="s">
         <v>364</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="121">
-      <c r="H121" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="122">
+      <c r="E122" s="1" t="n"/>
+      <c r="H122" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="I121" s="32" t="s">
+      <c r="I122" s="32" t="s">
         <v>366</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="122">
-      <c r="H122" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="123">
+      <c r="E123" s="1" t="n"/>
+      <c r="H123" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="I122" s="32" t="s">
+      <c r="I123" s="32" t="s">
         <v>368</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="123">
-      <c r="H123" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="124">
+      <c r="E124" s="1" t="n"/>
+      <c r="H124" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="I123" s="32" t="s">
+      <c r="I124" s="32" t="s">
         <v>370</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="124">
-      <c r="H124" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="125">
+      <c r="E125" s="1" t="n"/>
+      <c r="H125" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="I124" s="32" t="s">
+      <c r="I125" s="32" t="s">
         <v>372</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="125">
-      <c r="H125" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="126">
+      <c r="E126" s="1" t="n"/>
+      <c r="H126" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="I125" s="32" t="s">
+      <c r="I126" s="32" t="s">
         <v>374</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="126">
-      <c r="H126" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="127">
+      <c r="E127" s="1" t="n"/>
+      <c r="H127" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="I126" s="32" t="s">
+      <c r="I127" s="32" t="s">
         <v>376</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="127">
-      <c r="H127" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="128">
+      <c r="E128" s="1" t="n"/>
+      <c r="H128" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="I127" s="32" t="s">
+      <c r="I128" s="32" t="s">
         <v>378</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="128">
-      <c r="H128" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="129">
+      <c r="E129" s="1" t="n"/>
+      <c r="H129" s="35" t="s">
         <v>379</v>
       </c>
-      <c r="I128" s="32" t="s">
+      <c r="I129" s="32" t="s">
         <v>380</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="129">
-      <c r="H129" s="35" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="130">
+      <c r="E130" s="1" t="n"/>
+      <c r="H130" s="35" t="s">
         <v>381</v>
       </c>
-      <c r="I129" s="32" t="s">
+      <c r="I130" s="32" t="s">
         <v>382</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="130">
-      <c r="H130" s="35" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="131">
+      <c r="E131" s="1" t="n"/>
+      <c r="H131" s="35" t="s">
         <v>383</v>
       </c>
-      <c r="I130" s="32" t="s">
+      <c r="I131" s="32" t="s">
         <v>384</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="131">
-      <c r="H131" s="35" t="s">
+    <row hidden="false" ht="14" outlineLevel="0" r="132">
+      <c r="E132" s="1" t="n"/>
+      <c r="H132" s="35" t="s">
         <v>385</v>
       </c>
-      <c r="I131" s="32" t="s">
+      <c r="I132" s="32" t="s">
         <v>386</v>
       </c>
     </row>
-    <row hidden="false" ht="14" outlineLevel="0" r="132">
-      <c r="H132" s="35" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="133">
+      <c r="E133" s="1" t="n"/>
+      <c r="H133" s="35" t="s">
         <v>387</v>
       </c>
-      <c r="I132" s="32" t="s">
+      <c r="I133" s="32" t="s">
         <v>388</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="133">
-      <c r="H133" s="35" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="134">
+      <c r="E134" s="1" t="n"/>
+      <c r="H134" s="35" t="s">
         <v>389</v>
       </c>
-      <c r="I133" s="32" t="s">
+      <c r="I134" s="32" t="s">
         <v>390</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="134">
-      <c r="H134" s="35" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="135">
+      <c r="E135" s="1" t="n"/>
+      <c r="H135" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I134" s="32" t="s">
+      <c r="I135" s="32" t="s">
         <v>392</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="135">
-      <c r="H135" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="136">
+      <c r="E136" s="1" t="n"/>
+      <c r="H136" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="I135" s="32" t="s">
+      <c r="I136" s="32" t="s">
         <v>394</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="136">
-      <c r="H136" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="137">
+      <c r="E137" s="1" t="n"/>
+      <c r="H137" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="I136" s="32" t="s">
+      <c r="I137" s="32" t="s">
         <v>396</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="137">
-      <c r="H137" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="138">
+      <c r="E138" s="1" t="n"/>
+      <c r="H138" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="I137" s="32" t="s">
+      <c r="I138" s="32" t="s">
         <v>398</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="138">
-      <c r="H138" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="139">
+      <c r="E139" s="1" t="n"/>
+      <c r="H139" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="I138" s="32" t="s">
+      <c r="I139" s="32" t="s">
         <v>400</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="139">
-      <c r="H139" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="140">
+      <c r="E140" s="1" t="n"/>
+      <c r="H140" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="I139" s="32" t="s">
+      <c r="I140" s="32" t="s">
         <v>402</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="140">
-      <c r="H140" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="141">
+      <c r="E141" s="1" t="n"/>
+      <c r="H141" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I140" s="32" t="s">
+      <c r="I141" s="32" t="s">
         <v>404</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="141">
-      <c r="H141" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="142">
+      <c r="E142" s="1" t="n"/>
+      <c r="H142" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="I141" s="32" t="s">
+      <c r="I142" s="32" t="s">
         <v>406</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="142">
-      <c r="H142" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="143">
+      <c r="E143" s="1" t="n"/>
+      <c r="H143" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="I142" s="32" t="s">
+      <c r="I143" s="32" t="s">
         <v>408</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="143">
-      <c r="H143" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="144">
+      <c r="E144" s="1" t="n"/>
+      <c r="H144" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I143" s="32" t="s">
+      <c r="I144" s="32" t="s">
         <v>410</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="144">
-      <c r="H144" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="145">
+      <c r="E145" s="1" t="n"/>
+      <c r="H145" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I144" s="32" t="s">
+      <c r="I145" s="32" t="s">
         <v>412</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="145">
-      <c r="H145" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="146">
+      <c r="E146" s="1" t="n"/>
+      <c r="H146" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="I145" s="32" t="s">
+      <c r="I146" s="32" t="s">
         <v>414</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="146">
-      <c r="H146" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="147">
+      <c r="E147" s="1" t="n"/>
+      <c r="H147" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="I146" s="32" t="s">
+      <c r="I147" s="32" t="s">
         <v>416</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="147">
-      <c r="H147" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="148">
+      <c r="E148" s="1" t="n"/>
+      <c r="H148" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I147" s="32" t="s">
+      <c r="I148" s="32" t="s">
         <v>418</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="148">
-      <c r="H148" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="149">
+      <c r="E149" s="1" t="n"/>
+      <c r="H149" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="I148" s="32" t="s">
+      <c r="I149" s="32" t="s">
         <v>420</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="149">
-      <c r="H149" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="150">
+      <c r="E150" s="1" t="n"/>
+      <c r="H150" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I149" s="32" t="s">
+      <c r="I150" s="32" t="s">
         <v>422</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="150">
-      <c r="H150" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="151">
+      <c r="E151" s="1" t="n"/>
+      <c r="H151" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="I150" s="32" t="s">
+      <c r="I151" s="32" t="s">
         <v>424</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="151">
-      <c r="H151" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="152">
+      <c r="E152" s="1" t="n"/>
+      <c r="H152" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="I151" s="32" t="s">
+      <c r="I152" s="32" t="s">
         <v>426</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="152">
-      <c r="H152" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="153">
+      <c r="E153" s="1" t="n"/>
+      <c r="H153" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I152" s="32" t="s">
+      <c r="I153" s="32" t="s">
         <v>428</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="153">
-      <c r="H153" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="154">
+      <c r="E154" s="1" t="n"/>
+      <c r="H154" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="I153" s="32" t="s">
+      <c r="I154" s="32" t="s">
         <v>430</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="154">
-      <c r="H154" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="155">
+      <c r="E155" s="1" t="n"/>
+      <c r="H155" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I154" s="32" t="s">
+      <c r="I155" s="32" t="s">
         <v>432</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="155">
-      <c r="H155" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="156">
+      <c r="E156" s="1" t="n"/>
+      <c r="H156" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I155" s="32" t="s">
+      <c r="I156" s="32" t="s">
         <v>434</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="156">
-      <c r="H156" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="157">
+      <c r="E157" s="1" t="n"/>
+      <c r="H157" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="I156" s="32" t="s">
+      <c r="I157" s="32" t="s">
         <v>436</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="157">
-      <c r="H157" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="158">
+      <c r="E158" s="1" t="n"/>
+      <c r="H158" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I157" s="32" t="s">
+      <c r="I158" s="32" t="s">
         <v>438</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="158">
-      <c r="H158" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="159">
+      <c r="E159" s="1" t="n"/>
+      <c r="H159" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I158" s="32" t="s">
+      <c r="I159" s="32" t="s">
         <v>440</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="159">
-      <c r="H159" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="160">
+      <c r="E160" s="1" t="n"/>
+      <c r="H160" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I159" s="32" t="s">
+      <c r="I160" s="32" t="s">
         <v>442</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="160">
-      <c r="H160" s="1" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="161">
+      <c r="E161" s="1" t="n"/>
+      <c r="I161" s="32" t="s">
         <v>443</v>
       </c>
-      <c r="I160" s="32" t="s">
+    </row>
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="162">
+      <c r="E162" s="1" t="n"/>
+      <c r="I162" s="32" t="s">
         <v>444</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="161">
-      <c r="I161" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="163">
+      <c r="E163" s="1" t="n"/>
+      <c r="I163" s="32" t="s">
         <v>445</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="162">
-      <c r="I162" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="164">
+      <c r="E164" s="1" t="n"/>
+      <c r="I164" s="32" t="s">
         <v>446</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="163">
-      <c r="I163" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="165">
+      <c r="E165" s="1" t="n"/>
+      <c r="I165" s="32" t="s">
         <v>447</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="164">
-      <c r="I164" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="166">
+      <c r="E166" s="1" t="n"/>
+      <c r="I166" s="32" t="s">
         <v>448</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="165">
-      <c r="I165" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="167">
+      <c r="E167" s="1" t="n"/>
+      <c r="I167" s="32" t="s">
         <v>449</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="166">
-      <c r="I166" s="32" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="167">
-      <c r="I167" s="32" t="s">
-        <v>451</v>
-      </c>
-    </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="168">
+      <c r="E168" s="1" t="n"/>
       <c r="I168" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="169">
+      <c r="E169" s="1" t="n"/>
       <c r="I169" s="32" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="170">
+      <c r="E170" s="1" t="n"/>
+      <c r="I170" s="32" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row hidden="false" ht="14" outlineLevel="0" r="171">
+      <c r="E171" s="1" t="n"/>
+      <c r="I171" s="32" t="s">
         <v>452</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="170">
-      <c r="I170" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="172">
+      <c r="E172" s="1" t="n"/>
+      <c r="I172" s="32" t="s">
         <v>453</v>
       </c>
     </row>
-    <row hidden="false" ht="14" outlineLevel="0" r="171">
-      <c r="I171" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="173">
+      <c r="E173" s="1" t="n"/>
+      <c r="I173" s="32" t="s">
         <v>454</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="172">
-      <c r="I172" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="174">
+      <c r="E174" s="1" t="n"/>
+      <c r="I174" s="32" t="s">
         <v>455</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="173">
-      <c r="I173" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="175">
+      <c r="E175" s="1" t="n"/>
+      <c r="I175" s="32" t="s">
         <v>456</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="174">
-      <c r="I174" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="176">
+      <c r="E176" s="1" t="n"/>
+      <c r="I176" s="32" t="s">
         <v>457</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="175">
-      <c r="I175" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="177">
+      <c r="E177" s="1" t="n"/>
+      <c r="I177" s="32" t="s">
         <v>458</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="176">
-      <c r="I176" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="178">
+      <c r="E178" s="1" t="n"/>
+      <c r="I178" s="32" t="s">
         <v>459</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="177">
-      <c r="I177" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="179">
+      <c r="E179" s="1" t="n"/>
+      <c r="I179" s="32" t="s">
         <v>460</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="178">
-      <c r="I178" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="180">
+      <c r="E180" s="1" t="n"/>
+      <c r="I180" s="32" t="s">
         <v>461</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="179">
-      <c r="I179" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="181">
+      <c r="E181" s="1" t="n"/>
+      <c r="I181" s="32" t="s">
         <v>462</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="180">
-      <c r="I180" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="182">
+      <c r="E182" s="1" t="n"/>
+      <c r="I182" s="32" t="s">
         <v>463</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="181">
-      <c r="I181" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="183">
+      <c r="E183" s="1" t="n"/>
+      <c r="I183" s="32" t="s">
         <v>464</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="182">
-      <c r="I182" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="184">
+      <c r="E184" s="1" t="n"/>
+      <c r="I184" s="32" t="s">
         <v>465</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="183">
-      <c r="I183" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="185">
+      <c r="E185" s="1" t="n"/>
+      <c r="I185" s="32" t="s">
         <v>466</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="184">
-      <c r="I184" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="186">
+      <c r="E186" s="1" t="n"/>
+      <c r="I186" s="32" t="s">
         <v>467</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="185">
-      <c r="I185" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="187">
+      <c r="E187" s="1" t="n"/>
+      <c r="I187" s="32" t="s">
         <v>468</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="186">
-      <c r="I186" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="188">
+      <c r="E188" s="1" t="n"/>
+      <c r="I188" s="32" t="s">
         <v>469</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="187">
-      <c r="I187" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="189">
+      <c r="E189" s="1" t="n"/>
+      <c r="I189" s="32" t="s">
         <v>470</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="188">
-      <c r="I188" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="190">
+      <c r="E190" s="1" t="n"/>
+      <c r="I190" s="32" t="s">
         <v>471</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="189">
-      <c r="I189" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="191">
+      <c r="E191" s="1" t="n"/>
+      <c r="I191" s="32" t="s">
         <v>472</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="190">
-      <c r="I190" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="192">
+      <c r="E192" s="1" t="n"/>
+      <c r="I192" s="32" t="s">
         <v>473</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="191">
-      <c r="I191" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="193">
+      <c r="E193" s="1" t="n"/>
+      <c r="I193" s="32" t="s">
         <v>474</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="192">
-      <c r="I192" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="194">
+      <c r="E194" s="1" t="n"/>
+      <c r="I194" s="32" t="s">
         <v>475</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="193">
-      <c r="I193" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="195">
+      <c r="E195" s="1" t="n"/>
+      <c r="I195" s="32" t="s">
         <v>476</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="194">
-      <c r="I194" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="196">
+      <c r="E196" s="1" t="n"/>
+      <c r="I196" s="32" t="s">
         <v>477</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="195">
-      <c r="I195" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="197">
+      <c r="E197" s="1" t="n"/>
+      <c r="I197" s="32" t="s">
         <v>478</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="196">
-      <c r="I196" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="198">
+      <c r="E198" s="1" t="n"/>
+      <c r="I198" s="32" t="s">
         <v>479</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="197">
-      <c r="I197" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="199">
+      <c r="E199" s="1" t="n"/>
+      <c r="I199" s="32" t="s">
         <v>480</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="198">
-      <c r="I198" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="200">
+      <c r="E200" s="1" t="n"/>
+      <c r="I200" s="32" t="s">
         <v>481</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="199">
-      <c r="I199" s="32" t="s">
+    <row hidden="false" ht="14" outlineLevel="0" r="201">
+      <c r="E201" s="1" t="n"/>
+      <c r="I201" s="32" t="s">
         <v>482</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="200">
-      <c r="I200" s="32" t="s">
+    <row hidden="false" ht="14" outlineLevel="0" r="202">
+      <c r="E202" s="1" t="n"/>
+      <c r="I202" s="32" t="s">
         <v>483</v>
       </c>
     </row>
-    <row hidden="false" ht="14" outlineLevel="0" r="201">
-      <c r="I201" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="203">
+      <c r="E203" s="1" t="n"/>
+      <c r="I203" s="32" t="s">
         <v>484</v>
       </c>
     </row>
-    <row hidden="false" ht="14" outlineLevel="0" r="202">
-      <c r="I202" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="204">
+      <c r="E204" s="1" t="n"/>
+      <c r="I204" s="32" t="s">
         <v>485</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="203">
-      <c r="I203" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="205">
+      <c r="E205" s="1" t="n"/>
+      <c r="I205" s="32" t="s">
         <v>486</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="204">
-      <c r="I204" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="206">
+      <c r="E206" s="1" t="n"/>
+      <c r="I206" s="32" t="s">
         <v>487</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="205">
-      <c r="I205" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="207">
+      <c r="E207" s="1" t="n"/>
+      <c r="I207" s="32" t="s">
         <v>488</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="206">
-      <c r="I206" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="208">
+      <c r="E208" s="1" t="n"/>
+      <c r="I208" s="32" t="s">
         <v>489</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="207">
-      <c r="I207" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="209">
+      <c r="E209" s="1" t="n"/>
+      <c r="I209" s="32" t="s">
         <v>490</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="208">
-      <c r="I208" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="210">
+      <c r="E210" s="1" t="n"/>
+      <c r="I210" s="32" t="s">
         <v>491</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="209">
-      <c r="I209" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="211">
+      <c r="E211" s="1" t="n"/>
+      <c r="I211" s="32" t="s">
         <v>492</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="210">
-      <c r="I210" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="212">
+      <c r="E212" s="1" t="n"/>
+      <c r="I212" s="32" t="s">
         <v>493</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="211">
-      <c r="I211" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="213">
+      <c r="E213" s="1" t="n"/>
+      <c r="I213" s="32" t="s">
         <v>494</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="212">
-      <c r="I212" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="214">
+      <c r="E214" s="1" t="n"/>
+      <c r="I214" s="32" t="s">
         <v>495</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="213">
-      <c r="I213" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="215">
+      <c r="E215" s="1" t="n"/>
+      <c r="I215" s="32" t="s">
         <v>496</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="214">
-      <c r="I214" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="216">
+      <c r="E216" s="1" t="n"/>
+      <c r="I216" s="32" t="s">
         <v>497</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="215">
-      <c r="I215" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="217">
+      <c r="E217" s="1" t="n"/>
+      <c r="I217" s="32" t="s">
         <v>498</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="216">
-      <c r="I216" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="218">
+      <c r="E218" s="1" t="n"/>
+      <c r="I218" s="32" t="s">
         <v>499</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="217">
-      <c r="I217" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="219">
+      <c r="E219" s="1" t="n"/>
+      <c r="I219" s="32" t="s">
         <v>500</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="218">
-      <c r="I218" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="220">
+      <c r="E220" s="1" t="n"/>
+      <c r="I220" s="32" t="s">
         <v>501</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="219">
-      <c r="I219" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="221">
+      <c r="E221" s="1" t="n"/>
+      <c r="I221" s="32" t="s">
         <v>502</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="220">
-      <c r="I220" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="222">
+      <c r="E222" s="1" t="n"/>
+      <c r="I222" s="32" t="s">
         <v>503</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="221">
-      <c r="I221" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="223">
+      <c r="E223" s="1" t="n"/>
+      <c r="I223" s="32" t="s">
         <v>504</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="222">
-      <c r="I222" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="224">
+      <c r="E224" s="1" t="n"/>
+      <c r="I224" s="32" t="s">
         <v>505</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="223">
-      <c r="I223" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="225">
+      <c r="E225" s="1" t="n"/>
+      <c r="I225" s="32" t="s">
         <v>506</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="224">
-      <c r="I224" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="226">
+      <c r="E226" s="1" t="n"/>
+      <c r="I226" s="32" t="s">
         <v>507</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="225">
-      <c r="I225" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="227">
+      <c r="E227" s="1" t="n"/>
+      <c r="I227" s="32" t="s">
         <v>508</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="226">
-      <c r="I226" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="228">
+      <c r="E228" s="1" t="n"/>
+      <c r="I228" s="32" t="s">
         <v>509</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="227">
-      <c r="I227" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="229">
+      <c r="E229" s="1" t="n"/>
+      <c r="I229" s="32" t="s">
         <v>510</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="228">
-      <c r="I228" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="230">
+      <c r="E230" s="1" t="n"/>
+      <c r="I230" s="32" t="s">
         <v>511</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="229">
-      <c r="I229" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="231">
+      <c r="E231" s="1" t="n"/>
+      <c r="I231" s="32" t="s">
         <v>512</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="230">
-      <c r="I230" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="232">
+      <c r="E232" s="1" t="n"/>
+      <c r="I232" s="32" t="s">
         <v>513</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="231">
-      <c r="I231" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="233">
+      <c r="E233" s="1" t="n"/>
+      <c r="I233" s="32" t="s">
         <v>514</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="232">
-      <c r="I232" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="234">
+      <c r="E234" s="1" t="n"/>
+      <c r="I234" s="32" t="s">
         <v>515</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="233">
-      <c r="I233" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="235">
+      <c r="E235" s="1" t="n"/>
+      <c r="I235" s="32" t="s">
         <v>516</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="234">
-      <c r="I234" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="236">
+      <c r="E236" s="1" t="n"/>
+      <c r="I236" s="32" t="s">
         <v>517</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="235">
-      <c r="I235" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="237">
+      <c r="E237" s="1" t="n"/>
+      <c r="I237" s="32" t="s">
         <v>518</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="236">
-      <c r="I236" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="238">
+      <c r="E238" s="1" t="n"/>
+      <c r="I238" s="32" t="s">
         <v>519</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="237">
-      <c r="I237" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="239">
+      <c r="E239" s="1" t="n"/>
+      <c r="I239" s="32" t="s">
         <v>520</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="238">
-      <c r="I238" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="240">
+      <c r="E240" s="1" t="n"/>
+      <c r="I240" s="32" t="s">
         <v>521</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="239">
-      <c r="I239" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="241">
+      <c r="E241" s="1" t="n"/>
+      <c r="I241" s="32" t="s">
         <v>522</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="240">
-      <c r="I240" s="32" t="s">
+    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="242">
+      <c r="E242" s="1" t="n"/>
+      <c r="I242" s="32" t="s">
         <v>523</v>
       </c>
     </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="241">
-      <c r="I241" s="32" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="242">
-      <c r="I242" s="32" t="s">
-        <v>525</v>
-      </c>
-    </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="243">
+      <c r="E243" s="1" t="n"/>
       <c r="I243" s="32" t="n"/>
     </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="244">
+      <c r="E244" s="1" t="n"/>
       <c r="I244" s="32" t="n"/>
     </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="245">
+      <c r="E245" s="1" t="n"/>
       <c r="I245" s="32" t="n"/>
     </row>
     <row hidden="false" ht="13.8000001907349" outlineLevel="0" r="246">
+      <c r="E246" s="1" t="n"/>
       <c r="I246" s="32" t="n"/>
     </row>
   </sheetData>
@@ -17977,13 +18101,13 @@
   <sheetData>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="2">
       <c r="C2" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>526</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>527</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>528</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="3">
@@ -17994,7 +18118,7 @@
         <v>341</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="4">
@@ -18002,10 +18126,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="5">
@@ -18013,10 +18137,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="6">
@@ -18024,10 +18148,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="7">
@@ -18035,10 +18159,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="8">
@@ -18046,10 +18170,10 @@
         <v>17</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="9">
@@ -18057,10 +18181,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="10">
@@ -18068,10 +18192,10 @@
         <v>19</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="11">
@@ -18079,10 +18203,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="12">
@@ -18090,10 +18214,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="13">
@@ -18101,10 +18225,10 @@
         <v>22</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="14">
@@ -18112,10 +18236,10 @@
         <v>23</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="15">
@@ -18123,10 +18247,10 @@
         <v>24</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="16">
@@ -18134,10 +18258,10 @@
         <v>25</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="17">
@@ -18145,10 +18269,10 @@
         <v>26</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="18">
@@ -18156,10 +18280,10 @@
         <v>27</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="19">
@@ -18167,10 +18291,10 @@
         <v>28</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="20">
@@ -18178,10 +18302,10 @@
         <v>29</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="21">
@@ -18189,10 +18313,10 @@
         <v>30</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="22">
@@ -18200,7 +18324,7 @@
         <v>31</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="23">
@@ -18208,7 +18332,7 @@
         <v>32</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="24">
@@ -18216,7 +18340,7 @@
         <v>33</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="25">
@@ -18224,7 +18348,7 @@
         <v>34</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="26">
@@ -18232,7 +18356,7 @@
         <v>35</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="27">
@@ -18240,7 +18364,7 @@
         <v>36</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row hidden="false" ht="12.8000001907349" outlineLevel="0" r="28">
@@ -18685,106 +18809,106 @@
   <sheetData>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="37" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="39" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="39" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="39" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="41" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="39" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="39" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="39" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="39" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="39" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="39" t="n"/>
       <c r="B11" s="42" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="39" t="n"/>
       <c r="B12" s="42" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="39" t="n"/>
       <c r="B13" s="42" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="39" t="n"/>
       <c r="B14" s="42" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">

</xml_diff>